<commit_message>
se realiza validaciones y se sube la creacion de reportes de solicitud
</commit_message>
<xml_diff>
--- a/src/Views/assets/excel/reporte-almuerzos.xlsx
+++ b/src/Views/assets/excel/reporte-almuerzos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp-8.2.4\htdocs\sistema-medico\src\Views\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{774675ED-F8A0-4DEC-85E6-6FCBE4A15D88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23A7B25E-5F73-4D08-87FC-997A62F97A54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" xr2:uid="{0F4216FD-D022-4816-9ABF-EEC2162C73E1}"/>
   </bookViews>
@@ -39,14 +39,14 @@
     <t>#</t>
   </si>
   <si>
-    <t xml:space="preserve">INFORMACION </t>
+    <t>Relacion de Solicitudes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -61,6 +61,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial Black"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -98,25 +105,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -489,27 +499,27 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27" style="6" customWidth="1"/>
-    <col min="3" max="3" width="80.85546875" style="6" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" style="6" customWidth="1"/>
+    <col min="1" max="1" width="4" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27" style="4" customWidth="1"/>
+    <col min="3" max="3" width="80.85546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="2" t="s">
+      <c r="A1" s="6"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="2"/>
+      <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">

</xml_diff>